<commit_message>
Alien nomads log series is complete and can be embedded in the map now.
</commit_message>
<xml_diff>
--- a/data/design/RallyPuzzle.xlsx
+++ b/data/design/RallyPuzzle.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspaces\cosmodog\data\design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62439977-D395-4894-A7B9-22E82EAC705F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDFEB768-14A2-4D75-8A14-82AD30ECADC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{9E72EB8A-5F51-459F-96EB-DA12CADBE06F}"/>
   </bookViews>
@@ -256,7 +256,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -300,9 +300,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -321,7 +318,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -658,10 +655,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{310FC57A-8B23-4357-A4CF-B99ECCC05441}">
-  <dimension ref="K8:AS39"/>
+  <dimension ref="F8:AS39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q32" sqref="Q32"/>
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="43.5" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -741,7 +738,6 @@
     <row r="11" spans="15:41" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="Z11" s="2"/>
       <c r="AD11" s="2"/>
-      <c r="AI11" s="15"/>
       <c r="AJ11" s="12" t="s">
         <v>9</v>
       </c>
@@ -770,17 +766,15 @@
         <v>14</v>
       </c>
       <c r="AD12" s="2"/>
-      <c r="AI12" s="15"/>
-      <c r="AJ12" s="17" t="s">
+      <c r="AJ12" s="16" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="13" spans="15:41" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="AI13" s="15"/>
       <c r="AJ13" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="AK13" s="18"/>
+      <c r="AK13" s="17"/>
       <c r="AL13" s="2"/>
       <c r="AM13" s="9">
         <v>5</v>
@@ -793,7 +787,6 @@
       </c>
     </row>
     <row r="14" spans="15:41" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="AI14" s="15"/>
       <c r="AJ14" s="4" t="s">
         <v>3</v>
       </c>
@@ -808,14 +801,14 @@
       <c r="AH16" s="2">
         <v>29</v>
       </c>
-      <c r="AI16" s="21" t="s">
+      <c r="AI16" s="20" t="s">
         <v>31</v>
       </c>
       <c r="AJ16" s="12" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="11:45" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="6:45" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="AE17" s="9">
         <v>3</v>
       </c>
@@ -823,13 +816,13 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="11:45" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="6:45" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="AE18" s="9">
         <v>3</v>
       </c>
       <c r="AI18" s="2"/>
     </row>
-    <row r="19" spans="11:45" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="6:45" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="AE19" s="9">
         <v>3</v>
       </c>
@@ -837,7 +830,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="11:45" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="6:45" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="AE20" s="2"/>
       <c r="AF20" s="2"/>
       <c r="AG20" s="2"/>
@@ -846,21 +839,21 @@
       </c>
       <c r="AI20" s="2"/>
     </row>
-    <row r="21" spans="11:45" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="6:45" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="N21" s="9">
         <v>30</v>
       </c>
       <c r="AI21" s="2"/>
     </row>
-    <row r="22" spans="11:45" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="6:45" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="N22" s="2"/>
       <c r="AI22" s="2"/>
     </row>
-    <row r="23" spans="11:45" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="6:45" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="N23" s="2"/>
       <c r="AI23" s="2"/>
     </row>
-    <row r="24" spans="11:45" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="6:45" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="N24" s="2"/>
       <c r="AI24" s="2"/>
       <c r="AP24" s="1" t="s">
@@ -869,14 +862,14 @@
       <c r="AQ24" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AR24" s="19" t="s">
+      <c r="AR24" s="18" t="s">
         <v>29</v>
       </c>
       <c r="AS24" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="11:45" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="6:45" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="N25" s="2"/>
       <c r="AE25" s="2"/>
       <c r="AF25" s="12" t="s">
@@ -888,7 +881,7 @@
       <c r="AH25" s="11">
         <v>21</v>
       </c>
-      <c r="AI25" s="17" t="s">
+      <c r="AI25" s="16" t="s">
         <v>13</v>
       </c>
       <c r="AJ25" s="11">
@@ -918,7 +911,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="11:45" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="6:45" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="N26" s="2"/>
       <c r="AE26" s="2"/>
       <c r="AM26" s="2"/>
@@ -939,7 +932,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="11:45" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="6:45" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="N27" s="10" t="s">
         <v>20</v>
       </c>
@@ -960,18 +953,13 @@
         <v>8</v>
       </c>
       <c r="AS27" s="1">
-        <f t="shared" ref="AS26:AS28" si="0">AP27+AQ27-AR27</f>
+        <f t="shared" ref="AS27:AS28" si="0">AP27+AQ27-AR27</f>
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="11:45" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="K28" s="15"/>
-      <c r="L28" s="15"/>
-      <c r="M28" s="15"/>
+    <row r="28" spans="6:45" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F28" s="18"/>
       <c r="N28" s="2"/>
-      <c r="O28" s="15"/>
-      <c r="P28" s="15"/>
-      <c r="Q28" s="15"/>
       <c r="AE28" s="2"/>
       <c r="AM28" s="2"/>
       <c r="AO28" s="1" t="s">
@@ -991,20 +979,18 @@
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="11:45" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="K29" s="15"/>
+    <row r="29" spans="6:45" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="L29" s="2"/>
       <c r="M29" s="2"/>
       <c r="N29" s="4" t="s">
         <v>4</v>
       </c>
       <c r="O29" s="9">
+        <v>4</v>
+      </c>
+      <c r="P29" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="P29" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q29" s="15"/>
       <c r="AE29" s="2"/>
       <c r="AF29" s="2"/>
       <c r="AG29" s="2"/>
@@ -1019,8 +1005,7 @@
       <c r="AL29" s="2"/>
       <c r="AM29" s="2"/>
     </row>
-    <row r="30" spans="11:45" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="K30" s="15"/>
+    <row r="30" spans="6:45" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="L30" s="4" t="s">
         <v>3</v>
       </c>
@@ -1028,7 +1013,6 @@
       <c r="P30" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="Q30" s="15"/>
       <c r="V30" s="1" t="s">
         <v>27</v>
       </c>
@@ -1043,18 +1027,16 @@
       </c>
       <c r="AI30" s="2"/>
     </row>
-    <row r="31" spans="11:45" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="K31" s="15"/>
+    <row r="31" spans="6:45" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="L31" s="2"/>
       <c r="M31" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="N31" s="16" t="s">
+      <c r="N31" s="15" t="s">
         <v>5</v>
       </c>
       <c r="O31" s="2"/>
       <c r="P31" s="2"/>
-      <c r="Q31" s="15"/>
       <c r="U31" s="1" t="s">
         <v>35</v>
       </c>
@@ -1093,14 +1075,12 @@
       <c r="AL31" s="12"/>
       <c r="AM31" s="2"/>
     </row>
-    <row r="32" spans="11:45" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="K32" s="15"/>
+    <row r="32" spans="6:45" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="L32" s="9">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="N32" s="2"/>
       <c r="P32" s="2"/>
-      <c r="Q32" s="15"/>
       <c r="U32" s="1" t="s">
         <v>36</v>
       </c>
@@ -1120,29 +1100,22 @@
       <c r="AE32" s="2"/>
       <c r="AM32" s="2"/>
     </row>
-    <row r="33" spans="11:39" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="K33" s="15"/>
+    <row r="33" spans="12:39" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="L33" s="2"/>
       <c r="M33" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="N33" s="17" t="s">
+      <c r="N33" s="16" t="s">
         <v>37</v>
       </c>
       <c r="O33" s="2"/>
       <c r="P33" s="2"/>
-      <c r="Q33" s="15"/>
       <c r="AE33" s="2"/>
       <c r="AM33" s="2"/>
     </row>
-    <row r="34" spans="11:39" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="12:39" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="N34" s="2"/>
-      <c r="T34" s="15"/>
-      <c r="U34" s="15"/>
-      <c r="V34" s="15"/>
-      <c r="W34" s="22"/>
-      <c r="X34" s="15"/>
-      <c r="Y34" s="15"/>
+      <c r="W34" s="21"/>
       <c r="AE34" s="9">
         <v>3</v>
       </c>
@@ -1150,7 +1123,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="11:39" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="12:39" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="N35" s="2"/>
       <c r="T35" s="2"/>
       <c r="U35" s="9">
@@ -1180,15 +1153,15 @@
       <c r="AL35" s="2"/>
       <c r="AM35" s="2"/>
     </row>
-    <row r="36" spans="11:39" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="12:39" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="N36" s="2"/>
       <c r="T36" s="11"/>
       <c r="Y36" s="2"/>
-      <c r="AI36" s="20" t="s">
+      <c r="AI36" s="19" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="37" spans="11:39" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="12:39" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="N37" s="2"/>
       <c r="O37" s="2"/>
       <c r="P37" s="2"/>
@@ -1198,7 +1171,7 @@
         <v>20</v>
       </c>
       <c r="T37" s="2"/>
-      <c r="Y37" s="17" t="s">
+      <c r="Y37" s="16" t="s">
         <v>33</v>
       </c>
       <c r="Z37" s="9">
@@ -1214,11 +1187,11 @@
       <c r="AH37" s="2"/>
       <c r="AI37" s="2"/>
     </row>
-    <row r="38" spans="11:39" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="12:39" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="T38" s="2"/>
       <c r="Y38" s="2"/>
     </row>
-    <row r="39" spans="11:39" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="12:39" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="T39" s="2"/>
       <c r="U39" s="2"/>
       <c r="V39" s="2"/>

</xml_diff>

<commit_message>
Race puzzle is more refined now.
</commit_message>
<xml_diff>
--- a/data/design/RallyPuzzle.xlsx
+++ b/data/design/RallyPuzzle.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspaces\cosmodog\data\design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDFEB768-14A2-4D75-8A14-82AD30ECADC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA09DFFE-FC5C-4BD2-9BBC-30D057D0DDD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{9E72EB8A-5F51-459F-96EB-DA12CADBE06F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="40">
   <si>
     <t>7/7</t>
   </si>
@@ -171,6 +171,9 @@
   </si>
   <si>
     <t>3/6</t>
+  </si>
+  <si>
+    <t>3/3</t>
   </si>
 </sst>
 </file>
@@ -206,7 +209,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -243,6 +246,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -256,7 +271,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -319,6 +334,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="1" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -657,8 +681,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{310FC57A-8B23-4357-A4CF-B99ECCC05441}">
   <dimension ref="F8:AS39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+    <sheetView tabSelected="1" topLeftCell="I28" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="43.5" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -666,7 +690,7 @@
     <col min="1" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="8" spans="15:41" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="11:41" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="Z8" s="2"/>
       <c r="AA8" s="2">
         <v>16</v>
@@ -682,7 +706,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="15:41" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="11:41" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="O9" s="1">
         <v>30</v>
       </c>
@@ -698,7 +722,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="15:41" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="11:41" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="O10" s="3"/>
       <c r="P10" s="2"/>
       <c r="Q10" s="2"/>
@@ -735,7 +759,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="15:41" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="11:41" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="Z11" s="2"/>
       <c r="AD11" s="2"/>
       <c r="AJ11" s="12" t="s">
@@ -754,7 +778,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="15:41" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="11:41" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="Z12" s="2"/>
       <c r="AA12" s="2">
         <v>16</v>
@@ -770,7 +794,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="15:41" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="11:41" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="AJ13" s="12" t="s">
         <v>11</v>
       </c>
@@ -786,15 +810,60 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="15:41" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="11:41" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="P14" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q14" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="R14" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="S14" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="T14" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="U14" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="V14" s="15" t="s">
+        <v>5</v>
+      </c>
       <c r="AJ14" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="15:41" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="11:41" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K15" s="9">
+        <v>10</v>
+      </c>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="O15" s="2"/>
+      <c r="P15" s="2"/>
+      <c r="Q15" s="2"/>
+      <c r="R15" s="2"/>
+      <c r="S15" s="2"/>
+      <c r="T15" s="2"/>
+      <c r="U15" s="2"/>
+      <c r="V15" s="2"/>
+      <c r="W15" s="2"/>
+      <c r="X15" s="15" t="s">
+        <v>5</v>
+      </c>
       <c r="AJ15" s="2"/>
     </row>
-    <row r="16" spans="15:41" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="11:41" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="S16" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="X16" s="2"/>
       <c r="AE16" s="2"/>
       <c r="AF16" s="7"/>
       <c r="AG16" s="8"/>
@@ -809,6 +878,10 @@
       </c>
     </row>
     <row r="17" spans="6:45" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="S17" s="9">
+        <v>12</v>
+      </c>
+      <c r="X17" s="2"/>
       <c r="AE17" s="9">
         <v>3</v>
       </c>
@@ -817,12 +890,21 @@
       </c>
     </row>
     <row r="18" spans="6:45" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="X18" s="2"/>
       <c r="AE18" s="9">
         <v>3</v>
       </c>
       <c r="AI18" s="2"/>
     </row>
     <row r="19" spans="6:45" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Q19" s="2"/>
+      <c r="R19" s="2"/>
+      <c r="S19" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="T19" s="2"/>
+      <c r="U19" s="2"/>
+      <c r="X19" s="2"/>
       <c r="AE19" s="9">
         <v>3</v>
       </c>
@@ -831,6 +913,12 @@
       </c>
     </row>
     <row r="20" spans="6:45" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Q20" s="2"/>
+      <c r="R20" s="22"/>
+      <c r="S20" s="22"/>
+      <c r="T20" s="22"/>
+      <c r="U20" s="2"/>
+      <c r="X20" s="2"/>
       <c r="AE20" s="2"/>
       <c r="AF20" s="2"/>
       <c r="AG20" s="2"/>
@@ -841,16 +929,40 @@
     </row>
     <row r="21" spans="6:45" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="N21" s="9">
-        <v>30</v>
+        <v>10</v>
+      </c>
+      <c r="O21" s="2"/>
+      <c r="P21" s="2"/>
+      <c r="Q21" s="2"/>
+      <c r="R21" s="24"/>
+      <c r="S21" s="24"/>
+      <c r="T21" s="24"/>
+      <c r="U21" s="2"/>
+      <c r="V21" s="2"/>
+      <c r="W21" s="2"/>
+      <c r="X21" s="9">
+        <v>15</v>
       </c>
       <c r="AI21" s="2"/>
     </row>
     <row r="22" spans="6:45" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="N22" s="2"/>
+      <c r="Q22" s="2"/>
+      <c r="R22" s="22"/>
+      <c r="S22" s="22"/>
+      <c r="T22" s="22"/>
+      <c r="U22" s="2"/>
       <c r="AI22" s="2"/>
     </row>
     <row r="23" spans="6:45" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="N23" s="2"/>
+      <c r="Q23" s="2"/>
+      <c r="R23" s="2"/>
+      <c r="S23" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="T23" s="2"/>
+      <c r="U23" s="2"/>
       <c r="AI23" s="2"/>
     </row>
     <row r="24" spans="6:45" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>